<commit_message>
Updated Excel - Lookups
</commit_message>
<xml_diff>
--- a/example/UC.xlsx
+++ b/example/UC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmarau/University/Teaching/LiveSystems/PacoAutomationScript/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC47BC7-C8FD-9447-93F3-D9FAF8C196E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5981F949-ADE2-B64B-851F-7DFBD72838DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="664" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PacoDump" sheetId="2" r:id="rId1"/>
@@ -45,6 +45,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -207,8 +229,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-816]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -408,9 +431,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -452,6 +472,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7189,23 +7212,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+    <sheetView zoomScale="143" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="25" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="25" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="25" customWidth="1"/>
-    <col min="9" max="9" width="7.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="25" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="24" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="24" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="24" customWidth="1"/>
+    <col min="8" max="8" width="7.5" style="24" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="24" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -7281,73 +7304,73 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>50</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="27">
         <v>0</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="27">
         <v>100002</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="27">
         <v>2000</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="28" t="str">
+      <c r="K3" s="27" t="str">
         <f t="shared" ref="K3" si="1">PROPER(CONCATENATE(LEFT(B3,SEARCH(" ",B3)-1), " ", TRIM(RIGHT(SUBSTITUTE(B3," ",REPT(" ",LEN(B3))),LEN(B3)))))</f>
         <v>Nome Sicrano</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>50</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>0</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="27">
         <v>100003</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="27">
         <v>2000</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="28" t="str">
+      <c r="K4" s="27" t="str">
         <f t="shared" ref="K4" si="2">PROPER(CONCATENATE(LEFT(B4,SEARCH(" ",B4)-1), " ", TRIM(RIGHT(SUBSTITUTE(B4," ",REPT(" ",LEN(B4))),LEN(B4)))))</f>
         <v>Nome Beltrano</v>
       </c>
@@ -7360,52 +7383,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:AW48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="25" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="25" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="39.5" style="25" customWidth="1"/>
-    <col min="7" max="7" width="38.5" style="25" customWidth="1"/>
-    <col min="8" max="8" width="62.33203125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5" style="24" customWidth="1"/>
+    <col min="6" max="6" width="39.5" style="24" customWidth="1"/>
+    <col min="7" max="7" width="38.5" style="24" customWidth="1"/>
+    <col min="8" max="8" width="62.33203125" style="24" customWidth="1"/>
+    <col min="49" max="49" width="22.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>43</v>
       </c>
+      <c r="AW1" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>44</v>
       </c>
+      <c r="AW2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="33" t="b">
+      <c r="B3" s="32" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -7431,8 +7460,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="27" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37">
+    <row r="6" spans="1:49" s="26" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36">
         <v>44630</v>
       </c>
       <c r="B6" s="14">
@@ -7444,7 +7473,7 @@
       <c r="D6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="16" t="s">
@@ -7453,12 +7482,12 @@
       <c r="G6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="27" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38"/>
+    <row r="7" spans="1:49" s="26" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="37"/>
       <c r="B7" s="14">
         <v>2</v>
       </c>
@@ -7469,7 +7498,7 @@
       <c r="D7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="16" t="s">
@@ -7478,12 +7507,12 @@
       <c r="G7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="26" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35">
+    <row r="8" spans="1:49" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34">
         <f>A6+7</f>
         <v>44637</v>
       </c>
@@ -7497,7 +7526,7 @@
       <c r="D8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="19" t="s">
@@ -7508,8 +7537,8 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" s="26" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:49" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="35"/>
       <c r="B9" s="17">
         <v>2</v>
       </c>
@@ -7520,7 +7549,7 @@
       <c r="D9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="19" t="s">
@@ -7531,8 +7560,8 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37">
+    <row r="10" spans="1:49" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36">
         <f>A8+7</f>
         <v>44644</v>
       </c>
@@ -7546,7 +7575,7 @@
       <c r="D10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="16" t="s">
@@ -7556,8 +7585,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
+    <row r="11" spans="1:49" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="37"/>
       <c r="B11" s="14">
         <v>2</v>
       </c>
@@ -7568,7 +7597,7 @@
       <c r="D11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="16" t="s">
@@ -7578,8 +7607,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="35">
+    <row r="12" spans="1:49" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34">
         <f>A10+7</f>
         <v>44651</v>
       </c>
@@ -7593,7 +7622,7 @@
       <c r="D12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="19" t="s">
@@ -7604,8 +7633,8 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:49" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="35"/>
       <c r="B13" s="17">
         <v>2</v>
       </c>
@@ -7616,7 +7645,7 @@
       <c r="D13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="19" t="s">
@@ -7627,8 +7656,8 @@
       </c>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37">
+    <row r="14" spans="1:49" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="36">
         <f>A12+7</f>
         <v>44658</v>
       </c>
@@ -7642,7 +7671,7 @@
       <c r="D14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="16" t="s">
@@ -7652,8 +7681,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
+    <row r="15" spans="1:49" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="37"/>
       <c r="B15" s="14">
         <v>2</v>
       </c>
@@ -7664,7 +7693,7 @@
       <c r="D15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="16" t="s">
@@ -7674,39 +7703,39 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="35">
+    <row r="16" spans="1:49" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34">
         <f>A14+7</f>
         <v>44665</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="31">
         <v>0</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="18"/>
-      <c r="E16" s="31"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="19"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="32">
+    <row r="17" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="35"/>
+      <c r="B17" s="31">
         <v>0</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="31"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="19"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
     </row>
-    <row r="18" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37">
+    <row r="18" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="36">
         <f>A16+7</f>
         <v>44672</v>
       </c>
@@ -7720,7 +7749,7 @@
       <c r="D18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F18" s="16" t="s">
@@ -7730,8 +7759,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="38"/>
+    <row r="19" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="37"/>
       <c r="B19" s="14">
         <v>2</v>
       </c>
@@ -7742,7 +7771,7 @@
       <c r="D19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="16" t="s">
@@ -7752,39 +7781,39 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="35">
+    <row r="20" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="34">
         <f>A18+7</f>
         <v>44679</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <v>0</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="31" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="18"/>
-      <c r="E20" s="31"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="19"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="32">
+    <row r="21" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="35"/>
+      <c r="B21" s="31">
         <v>0</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="31" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="18"/>
-      <c r="E21" s="31"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="19"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37">
+    <row r="22" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="36">
         <f>A20+7</f>
         <v>44686</v>
       </c>
@@ -7798,7 +7827,7 @@
       <c r="D22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="16" t="s">
@@ -7808,8 +7837,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
+    <row r="23" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="37"/>
       <c r="B23" s="14">
         <v>2</v>
       </c>
@@ -7820,7 +7849,7 @@
       <c r="D23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="16" t="s">
@@ -7830,8 +7859,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="35">
+    <row r="24" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="34">
         <f>A22+7</f>
         <v>44693</v>
       </c>
@@ -7845,7 +7874,7 @@
       <c r="D24" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="19" t="s">
@@ -7856,8 +7885,8 @@
       </c>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="35"/>
       <c r="B25" s="17">
         <v>2</v>
       </c>
@@ -7868,7 +7897,7 @@
       <c r="D25" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F25" s="19" t="s">
@@ -7879,8 +7908,8 @@
       </c>
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37">
+    <row r="26" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="36">
         <f>A24+7</f>
         <v>44700</v>
       </c>
@@ -7894,7 +7923,7 @@
       <c r="D26" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="16" t="s">
@@ -7904,8 +7933,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="38"/>
+    <row r="27" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="37"/>
       <c r="B27" s="14">
         <v>2</v>
       </c>
@@ -7916,7 +7945,7 @@
       <c r="D27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="16" t="s">
@@ -7926,8 +7955,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35">
+    <row r="28" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="34">
         <f>A26+14</f>
         <v>44714</v>
       </c>
@@ -7941,7 +7970,7 @@
       <c r="D28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="19" t="s">
@@ -7952,8 +7981,8 @@
       </c>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
+    <row r="29" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="35"/>
       <c r="B29" s="17">
         <v>2</v>
       </c>
@@ -7964,7 +7993,7 @@
       <c r="D29" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F29" s="19" t="s">
@@ -7975,8 +8004,8 @@
       </c>
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37">
+    <row r="30" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="36">
         <f>A28</f>
         <v>44714</v>
       </c>
@@ -7990,7 +8019,7 @@
       <c r="D30" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="16" t="s">
@@ -8000,8 +8029,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="38"/>
+    <row r="31" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="37"/>
       <c r="B31" s="14">
         <v>2</v>
       </c>
@@ -8012,7 +8041,7 @@
       <c r="D31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F31" s="16" t="s">
@@ -8022,8 +8051,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="35">
+    <row r="32" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34">
         <f>A30+7</f>
         <v>44721</v>
       </c>
@@ -8037,7 +8066,7 @@
       <c r="D32" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F32" s="19" t="s">
@@ -8048,8 +8077,8 @@
       </c>
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
+    <row r="33" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="35"/>
       <c r="B33" s="17">
         <v>2</v>
       </c>
@@ -8060,7 +8089,7 @@
       <c r="D33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="30" t="s">
         <v>25</v>
       </c>
       <c r="F33" s="19" t="s">
@@ -8071,37 +8100,37 @@
       </c>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37">
+    <row r="34" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="36">
         <f>A32+7</f>
         <v>44728</v>
       </c>
-      <c r="B34" s="34">
+      <c r="B34" s="33">
         <v>0</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="33" t="s">
         <v>28</v>
       </c>
       <c r="D34" s="15"/>
-      <c r="E34" s="31"/>
+      <c r="E34" s="30"/>
       <c r="F34" s="16"/>
       <c r="G34" s="21"/>
     </row>
-    <row r="35" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="38"/>
-      <c r="B35" s="34">
+    <row r="35" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="37"/>
+      <c r="B35" s="33">
         <v>0</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="33" t="s">
         <v>28</v>
       </c>
       <c r="D35" s="15"/>
-      <c r="E35" s="31"/>
+      <c r="E35" s="30"/>
       <c r="F35" s="16"/>
       <c r="G35" s="21"/>
     </row>
-    <row r="36" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="35">
+    <row r="36" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="34">
         <f>A34+7</f>
         <v>44735</v>
       </c>
@@ -8115,7 +8144,7 @@
       <c r="D36" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="19" t="s">
         <v>45</v>
       </c>
@@ -8124,8 +8153,8 @@
       </c>
       <c r="H36" s="20"/>
     </row>
-    <row r="37" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
+    <row r="37" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="35"/>
       <c r="B37" s="17">
         <v>2</v>
       </c>
@@ -8136,7 +8165,7 @@
       <c r="D37" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="31"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="19" t="s">
         <v>45</v>
       </c>
@@ -8145,8 +8174,8 @@
       </c>
       <c r="H37" s="20"/>
     </row>
-    <row r="38" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37">
+    <row r="38" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="36">
         <f>A36+7</f>
         <v>44742</v>
       </c>
@@ -8160,7 +8189,7 @@
       <c r="D38" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="16" t="s">
         <v>45</v>
       </c>
@@ -8168,8 +8197,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="30" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="38"/>
+    <row r="39" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="37"/>
       <c r="B39" s="14">
         <v>2</v>
       </c>
@@ -8180,7 +8209,7 @@
       <c r="D39" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="31"/>
+      <c r="E39" s="30"/>
       <c r="F39" s="16" t="s">
         <v>45</v>
       </c>
@@ -8188,8 +8217,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="35">
+    <row r="40" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="34">
         <f>A38+7</f>
         <v>44749</v>
       </c>
@@ -8203,7 +8232,7 @@
       <c r="D40" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="31"/>
+      <c r="E40" s="30"/>
       <c r="F40" s="19" t="s">
         <v>45</v>
       </c>
@@ -8212,8 +8241,8 @@
       </c>
       <c r="H40" s="20"/>
     </row>
-    <row r="41" spans="1:8" s="29" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
+    <row r="41" spans="1:8" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="35"/>
       <c r="B41" s="17">
         <v>2</v>
       </c>
@@ -8224,7 +8253,7 @@
       <c r="D41" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="31"/>
+      <c r="E41" s="30"/>
       <c r="F41" s="19" t="s">
         <v>45</v>
       </c>
@@ -8265,17 +8294,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A36:A37"/>
@@ -8283,7 +8301,23 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{1725F561-21A9-A14F-880B-52AB8C1657AE}">
+      <formula1>$AW$1:$AW$2</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -8293,8 +8327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AN30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8302,132 +8336,135 @@
     <col min="1" max="1" width="7.83203125" style="22" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="9" customWidth="1"/>
     <col min="3" max="20" width="11.1640625" style="9" customWidth="1"/>
-    <col min="21" max="40" width="10" style="9" customWidth="1"/>
+    <col min="21" max="32" width="10.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="40" width="10" style="9" customWidth="1"/>
     <col min="41" max="45" width="10.83203125" style="9" customWidth="1"/>
     <col min="46" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="23" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="24">
+      <c r="B1" s="39"/>
+      <c r="C1" s="41" cm="1">
+        <f t="array" ref="C1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(C2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(C2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(C2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44630</v>
       </c>
-      <c r="D1" s="24">
+      <c r="D1" s="41" cm="1">
+        <f t="array" ref="D1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(D2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(D2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(D2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44630</v>
       </c>
-      <c r="E1" s="24">
-        <f t="shared" ref="E1:L1" si="0">C1+7</f>
+      <c r="E1" s="41" cm="1">
+        <f t="array" ref="E1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(E2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(E2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(E2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44637</v>
       </c>
-      <c r="F1" s="24">
-        <f t="shared" si="0"/>
+      <c r="F1" s="41" cm="1">
+        <f t="array" ref="F1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(F2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(F2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(F2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44637</v>
       </c>
-      <c r="G1" s="24">
-        <f t="shared" si="0"/>
+      <c r="G1" s="41" cm="1">
+        <f t="array" ref="G1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(G2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(G2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(G2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44644</v>
       </c>
-      <c r="H1" s="24">
-        <f t="shared" si="0"/>
+      <c r="H1" s="41" cm="1">
+        <f t="array" ref="H1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(H2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(H2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(H2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44644</v>
       </c>
-      <c r="I1" s="24">
-        <f t="shared" si="0"/>
+      <c r="I1" s="41" cm="1">
+        <f t="array" ref="I1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(I2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(I2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(I2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44651</v>
       </c>
-      <c r="J1" s="24">
-        <f t="shared" si="0"/>
+      <c r="J1" s="41" cm="1">
+        <f t="array" ref="J1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(J2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(J2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(J2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44651</v>
       </c>
-      <c r="K1" s="24">
-        <f t="shared" si="0"/>
+      <c r="K1" s="41" cm="1">
+        <f t="array" ref="K1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(K2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(K2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(K2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44658</v>
       </c>
-      <c r="L1" s="24">
-        <f t="shared" si="0"/>
+      <c r="L1" s="41" cm="1">
+        <f t="array" ref="L1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(L2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(L2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(L2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44658</v>
       </c>
-      <c r="M1" s="24">
-        <f>K1+14</f>
+      <c r="M1" s="41" cm="1">
+        <f t="array" ref="M1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(M2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(M2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(M2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44672</v>
       </c>
-      <c r="N1" s="24">
-        <f>L1+14</f>
+      <c r="N1" s="41" cm="1">
+        <f t="array" ref="N1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(N2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(N2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(N2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44672</v>
       </c>
-      <c r="O1" s="24">
-        <f>M1+14</f>
+      <c r="O1" s="41" cm="1">
+        <f t="array" ref="O1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(O2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(O2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(O2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44686</v>
       </c>
-      <c r="P1" s="24">
-        <f>N1+14</f>
+      <c r="P1" s="41" cm="1">
+        <f t="array" ref="P1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(P2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(P2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(P2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44686</v>
       </c>
-      <c r="Q1" s="24">
-        <f>O1+7</f>
+      <c r="Q1" s="41" cm="1">
+        <f t="array" ref="Q1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(Q2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(Q2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(Q2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44693</v>
       </c>
-      <c r="R1" s="24">
-        <f>P1+7</f>
+      <c r="R1" s="41" cm="1">
+        <f t="array" ref="R1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(R2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(R2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(R2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44693</v>
       </c>
-      <c r="S1" s="24">
-        <f>Q1+7</f>
+      <c r="S1" s="41" cm="1">
+        <f t="array" ref="S1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(S2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(S2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(S2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44700</v>
       </c>
-      <c r="T1" s="24">
-        <f>R1+7</f>
+      <c r="T1" s="41" cm="1">
+        <f t="array" ref="T1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(T2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(T2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(T2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44700</v>
       </c>
-      <c r="U1" s="24">
-        <f>S1+14</f>
+      <c r="U1" s="41" cm="1">
+        <f t="array" ref="U1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(U2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(U2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(U2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44714</v>
       </c>
-      <c r="V1" s="24">
-        <f>T1+14</f>
+      <c r="V1" s="41" cm="1">
+        <f t="array" ref="V1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(V2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(V2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(V2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44714</v>
       </c>
-      <c r="W1" s="24">
-        <f>U1</f>
+      <c r="W1" s="41" cm="1">
+        <f t="array" ref="W1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(W2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(W2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(W2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44714</v>
       </c>
-      <c r="X1" s="24">
-        <f>V1</f>
+      <c r="X1" s="41" cm="1">
+        <f t="array" ref="X1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(X2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(X2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(X2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44714</v>
       </c>
-      <c r="Y1" s="24">
-        <f>W1+7</f>
+      <c r="Y1" s="41" cm="1">
+        <f t="array" ref="Y1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(Y2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(Y2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(Y2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44721</v>
       </c>
-      <c r="Z1" s="24">
-        <f>X1+7</f>
+      <c r="Z1" s="41" cm="1">
+        <f t="array" ref="Z1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(Z2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(Z2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(Z2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44721</v>
       </c>
-      <c r="AA1" s="24">
-        <f>Y1+14</f>
+      <c r="AA1" s="41" cm="1">
+        <f t="array" ref="AA1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(AA2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(AA2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(AA2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44735</v>
       </c>
-      <c r="AB1" s="24">
-        <f>Z1+14</f>
+      <c r="AB1" s="41" cm="1">
+        <f t="array" ref="AB1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(AB2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(AB2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(AB2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44735</v>
       </c>
-      <c r="AC1" s="24">
-        <f>AA1+7</f>
+      <c r="AC1" s="41" cm="1">
+        <f t="array" ref="AC1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(AC2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(AC2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(AC2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44742</v>
       </c>
-      <c r="AD1" s="24">
-        <f>AB1+7</f>
+      <c r="AD1" s="41" cm="1">
+        <f t="array" ref="AD1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(AD2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(AD2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(AD2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44742</v>
       </c>
-      <c r="AE1" s="24">
-        <f>AC1+7</f>
+      <c r="AE1" s="41" cm="1">
+        <f t="array" ref="AE1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(AE2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(AE2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(AE2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44749</v>
       </c>
-      <c r="AF1" s="24">
-        <f>AD1+7</f>
+      <c r="AF1" s="41" cm="1">
+        <f t="array" ref="AF1">IF(INDEX(Planeamento!$A$6:$A$200,MATCH(AF2,Planeamento!$C$6:$C$200,0)) = 0, INDEX(Planeamento!$A$6:$A$200,MATCH(AF2,Planeamento!$C$6:$C$200,0)-1), INDEX(Planeamento!$A$6:$A$200,MATCH(AF2,Planeamento!$C$6:$C$200,0)))</f>
         <v>44749</v>
       </c>
       <c r="AG1" s="6"/>
@@ -8440,8 +8477,8 @@
       <c r="AN1" s="6"/>
     </row>
     <row r="2" spans="1:40" s="23" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="8">
         <v>1</v>
       </c>

</xml_diff>